<commit_message>
created comparison file for susvsink metagomics sorted results
</commit_message>
<xml_diff>
--- a/analyses/metagomics/susvsink/susvsink-metagomics-go-comparison.xlsx
+++ b/analyses/metagomics/susvsink/susvsink-metagomics-go-comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/metagomics/susvsink/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B29A8A10-A650-ED47-9E3F-2B5815E8F88D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172C9FC3-021F-B745-8006-7030CA8417BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="5560" windowWidth="26040" windowHeight="14940" xr2:uid="{F273551E-9FEB-5548-BBD9-F9B9F48DA798}"/>
+    <workbookView xWindow="2980" yWindow="3860" windowWidth="26040" windowHeight="14940" xr2:uid="{F273551E-9FEB-5548-BBD9-F9B9F48DA798}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,98 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>JA2</t>
+  </si>
+  <si>
+    <t>Sus/Sink</t>
+  </si>
+  <si>
+    <t>JA14</t>
+  </si>
+  <si>
+    <t>264+265</t>
+  </si>
+  <si>
+    <t>268+269</t>
+  </si>
+  <si>
+    <t>Depth (m)</t>
+  </si>
+  <si>
+    <t>sus</t>
+  </si>
+  <si>
+    <t>sink</t>
+  </si>
+  <si>
+    <t>% GO spectra - biological process</t>
+  </si>
+  <si>
+    <t>photosynthesis</t>
+  </si>
+  <si>
+    <t>organic substance metabolic process</t>
+  </si>
+  <si>
+    <t>nitrogen compound metabolic process</t>
+  </si>
+  <si>
+    <t>transport</t>
+  </si>
+  <si>
+    <t>protein metabolic process</t>
+  </si>
+  <si>
+    <t>% GO spectra - cellular component</t>
+  </si>
+  <si>
+    <t>cytosolic</t>
+  </si>
+  <si>
+    <t>chloroplast</t>
+  </si>
+  <si>
+    <t>membrane</t>
+  </si>
+  <si>
+    <t>cell wall</t>
+  </si>
+  <si>
+    <t>% GO spectra - molecular function</t>
+  </si>
+  <si>
+    <t>protein binding</t>
+  </si>
+  <si>
+    <t>catalytic function</t>
+  </si>
+  <si>
+    <t>organic cyclic compound binding</t>
+  </si>
+  <si>
+    <t>metal ion binding</t>
+  </si>
+  <si>
+    <t>nucleotide binding</t>
+  </si>
+  <si>
+    <t>*this squares with Bergauer et al 2018, but not very specific in terms of substrate!</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -34,16 +123,57 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -51,12 +181,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,12 +539,306 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD53EBE-D2D2-9B43-AAF1-36618F3EEAE2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:BJ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="14.6640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="10"/>
+    <col min="8" max="8" width="17.1640625" style="10" customWidth="1"/>
+    <col min="9" max="14" width="10.83203125" style="10"/>
+    <col min="15" max="15" width="19.83203125" style="10" customWidth="1"/>
+    <col min="16" max="62" width="10.83203125" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:62" s="1" customFormat="1" ht="29" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6"/>
+      <c r="AM1" s="6"/>
+      <c r="AN1" s="6"/>
+      <c r="AO1" s="6"/>
+      <c r="AP1" s="6"/>
+      <c r="AQ1" s="6"/>
+      <c r="AR1" s="6"/>
+      <c r="AS1" s="6"/>
+      <c r="AT1" s="6"/>
+      <c r="AU1" s="6"/>
+      <c r="AV1" s="6"/>
+      <c r="AW1" s="6"/>
+      <c r="AX1" s="6"/>
+      <c r="AY1" s="6"/>
+      <c r="AZ1" s="6"/>
+      <c r="BA1" s="6"/>
+      <c r="BB1" s="6"/>
+      <c r="BC1" s="6"/>
+      <c r="BD1" s="6"/>
+      <c r="BE1" s="6"/>
+      <c r="BF1" s="6"/>
+      <c r="BG1" s="6"/>
+      <c r="BH1" s="6"/>
+      <c r="BI1" s="6"/>
+      <c r="BJ1" s="6"/>
+    </row>
+    <row r="2" spans="1:62" s="2" customFormat="1" ht="32">
+      <c r="D2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="9"/>
+      <c r="AO2" s="9"/>
+      <c r="AP2" s="9"/>
+      <c r="AQ2" s="9"/>
+      <c r="AR2" s="9"/>
+      <c r="AS2" s="9"/>
+      <c r="AT2" s="9"/>
+      <c r="AU2" s="9"/>
+      <c r="AV2" s="9"/>
+      <c r="AW2" s="9"/>
+      <c r="AX2" s="9"/>
+      <c r="AY2" s="9"/>
+      <c r="AZ2" s="9"/>
+      <c r="BA2" s="9"/>
+      <c r="BB2" s="9"/>
+      <c r="BC2" s="9"/>
+      <c r="BD2" s="9"/>
+      <c r="BE2" s="9"/>
+      <c r="BF2" s="9"/>
+      <c r="BG2" s="9"/>
+      <c r="BH2" s="9"/>
+      <c r="BI2" s="9"/>
+      <c r="BJ2" s="9"/>
+    </row>
+    <row r="3" spans="1:62">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.119554204660587</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.17527862208713199</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0.110097939885173</v>
+      </c>
+      <c r="G3" s="10">
+        <v>7.1597433299560906E-2</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0.11448834853090099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:62">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>965</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0.13043478260869501</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0.115942028985507</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0.21014492753623101</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:62">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>94</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="11">
+        <v>4.9001820000000001E-2</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0.1215971</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.10163339</v>
+      </c>
+      <c r="G5" s="10">
+        <v>6.5335749999999998E-2</v>
+      </c>
+      <c r="H5" s="10">
+        <v>4.9001820000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:62">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>965</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="10">
+        <v>9.1491308325708997E-4</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.18389752973467499</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.161939615736505</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0.103385178408051</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0.132662397072278</v>
+      </c>
+    </row>
+    <row r="9" spans="1:62">
+      <c r="E9" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:Q1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
restructured metagomics tax reports
</commit_message>
<xml_diff>
--- a/analyses/metagomics/susvsink/susvsink-metagomics-go-comparison.xlsx
+++ b/analyses/metagomics/susvsink/susvsink-metagomics-go-comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/metagomics/susvsink/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172C9FC3-021F-B745-8006-7030CA8417BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3776825-C644-1B4B-AAFB-D0E1ABCDA174}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="3860" windowWidth="26040" windowHeight="14940" xr2:uid="{F273551E-9FEB-5548-BBD9-F9B9F48DA798}"/>
+    <workbookView xWindow="2540" yWindow="3520" windowWidth="26040" windowHeight="14940" xr2:uid="{F273551E-9FEB-5548-BBD9-F9B9F48DA798}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -749,6 +749,18 @@
       <c r="H3" s="10">
         <v>0.11448834853090099</v>
       </c>
+      <c r="I3" s="10">
+        <v>7.66632894292468E-2</v>
+      </c>
+      <c r="J3" s="10">
+        <v>6.4842958459979699E-2</v>
+      </c>
+      <c r="K3" s="10">
+        <v>0.18034447821681801</v>
+      </c>
+      <c r="L3" s="10">
+        <v>5.3698074974670697E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:62">
       <c r="A4" t="s">
@@ -775,6 +787,18 @@
       <c r="H4" s="10">
         <v>0</v>
       </c>
+      <c r="I4" s="10">
+        <v>0.123188405797101</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0.108695652173913</v>
+      </c>
+      <c r="K4" s="10">
+        <v>0.137681159420289</v>
+      </c>
+      <c r="L4" s="10">
+        <v>0.123188405797101</v>
+      </c>
     </row>
     <row r="5" spans="1:62">
       <c r="A5" t="s">
@@ -801,6 +825,18 @@
       <c r="H5" s="10">
         <v>4.9001820000000001E-2</v>
       </c>
+      <c r="I5" s="10">
+        <v>7.8039929999999993E-2</v>
+      </c>
+      <c r="J5" s="10">
+        <v>5.4446460000000002E-2</v>
+      </c>
+      <c r="K5" s="10">
+        <v>8.5299459999999994E-2</v>
+      </c>
+      <c r="L5" s="10">
+        <v>4.9001820000000001E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:62">
       <c r="A6" t="s">
@@ -826,6 +862,18 @@
       </c>
       <c r="H6" s="10">
         <v>0.132662397072278</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0.13357731</v>
+      </c>
+      <c r="J6" s="10">
+        <v>8.6916740000000006E-2</v>
+      </c>
+      <c r="K6" s="10">
+        <v>0.11619396</v>
+      </c>
+      <c r="L6" s="10">
+        <v>9.2406219999999997E-2</v>
       </c>
     </row>
     <row r="9" spans="1:62">
@@ -840,5 +888,6 @@
     <mergeCell ref="M1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added unipept analyses for sno peps
</commit_message>
<xml_diff>
--- a/analyses/metagomics/susvsink/susvsink-metagomics-go-comparison.xlsx
+++ b/analyses/metagomics/susvsink/susvsink-metagomics-go-comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/metagomics/susvsink/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CD8680-4C21-8A47-96DC-ECBF67BCA965}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C80A297-2DB8-A843-BA90-6CABFD78C6FD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="25600" windowHeight="14640" xr2:uid="{F273551E-9FEB-5548-BBD9-F9B9F48DA798}"/>
+    <workbookView xWindow="2940" yWindow="5820" windowWidth="26040" windowHeight="14940" xr2:uid="{F273551E-9FEB-5548-BBD9-F9B9F48DA798}"/>
   </bookViews>
   <sheets>
     <sheet name="comparison" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,18 @@
     <sheet name="264+265" sheetId="4" r:id="rId4"/>
     <sheet name="268+269" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">comparison!$B$3:$B$6</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">comparison!$L$3:$L$6</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">comparison!$B$3:$B$6</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">comparison!$L$3:$L$6</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">comparison!$B$3:$B$6</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">comparison!$L$3:$L$6</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">comparison!$B$3:$B$6</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">comparison!$L$3:$L$6</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">comparison!$B$3:$B$6</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">comparison!$L$3:$L$6</definedName>
+  </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -231,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -275,6 +287,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -322,7 +337,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -341,25 +356,36 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>% spectra cytosolic</c:v>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00B050"/>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -371,15 +397,16 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -391,6 +418,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -398,10 +426,8 @@
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -413,6 +439,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -420,10 +447,8 @@
                   <a:lumMod val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -434,28 +459,6 @@
             </c:extLst>
           </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="9.1180227471566053E-2"/>
-                  <c:y val="-5.8755832604257804E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-2DA9-3841-A994-3EDB36086A42}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -470,9 +473,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="bg1"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -482,30 +488,32 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="ctr"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:round/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -556,17 +564,115 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1693857887"/>
+        <c:axId val="1789211807"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1693857887"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1789211807"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1789211807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1693857887"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -589,8 +695,8 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -678,7 +784,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -697,56 +803,69 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>% spectra membrane associated</c:v>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00B050"/>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-442D-7A43-B0AD-51099CEEE27C}"/>
+                <c16:uniqueId val="{00000001-5089-034C-83A7-365557DCE498}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-442D-7A43-B0AD-51099CEEE27C}"/>
+                <c16:uniqueId val="{00000003-5089-034C-83A7-365557DCE498}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -754,21 +873,20 @@
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-442D-7A43-B0AD-51099CEEE27C}"/>
+                <c16:uniqueId val="{00000005-5089-034C-83A7-365557DCE498}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
@@ -776,16 +894,14 @@
                   <a:lumMod val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-442D-7A43-B0AD-51099CEEE27C}"/>
+                <c16:uniqueId val="{00000007-5089-034C-83A7-365557DCE498}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -804,9 +920,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="bg1"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -816,30 +935,32 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="ctr"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:round/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -885,22 +1006,122 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-442D-7A43-B0AD-51099CEEE27C}"/>
+              <c16:uniqueId val="{00000008-5089-034C-83A7-365557DCE498}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1693857887"/>
+        <c:axId val="1789211807"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1693857887"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1789211807"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1789211807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1693857887"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -923,8 +1144,8 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1065,7 +1286,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1122,7 +1343,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1173,13 +1394,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1190,19 +1404,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -1240,7 +1447,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -1283,23 +1490,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1404,8 +1610,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1537,20 +1743,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1584,7 +1789,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1641,7 +1846,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1692,13 +1897,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1709,19 +1907,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -1759,7 +1950,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -1802,23 +1993,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1923,8 +2113,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2056,20 +2246,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2155,10 +2344,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19758545-4A6D-7C42-A210-C2A372C7874F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3715D5B-DC99-F84A-B07B-7EDCA328F4AB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2483,7 +2672,7 @@
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2511,9 +2700,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" s="1" customFormat="1" ht="29" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="19"/>
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3047,10 +3237,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="F1:K1"/>
     <mergeCell ref="L1:R1"/>
     <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
copied dno pep AA calc to propeps excel sheet, all looking good
</commit_message>
<xml_diff>
--- a/analyses/metagomics/susvsink/susvsink-metagomics-go-comparison.xlsx
+++ b/analyses/metagomics/susvsink/susvsink-metagomics-go-comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/metagomics/susvsink/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C80A297-2DB8-A843-BA90-6CABFD78C6FD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B8F247-6777-BD46-9ABC-68FEB80D7AB2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="5820" windowWidth="26040" windowHeight="14940" xr2:uid="{F273551E-9FEB-5548-BBD9-F9B9F48DA798}"/>
+    <workbookView xWindow="5840" yWindow="2280" windowWidth="26040" windowHeight="14660" xr2:uid="{F273551E-9FEB-5548-BBD9-F9B9F48DA798}"/>
   </bookViews>
   <sheets>
     <sheet name="comparison" sheetId="1" r:id="rId1"/>

</xml_diff>